<commit_message>
Minor modifications to custom schema
</commit_message>
<xml_diff>
--- a/optoelectronics/solar_cells_efficiency_tables/efficiency_tables.archive.xlsx
+++ b/optoelectronics/solar_cells_efficiency_tables/efficiency_tables.archive.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepem\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pepe_marquez\AreaE\AreaE_use-cases\optoelectronics\solar_cells_efficiency_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BF693F-273F-4429-8B03-11E78B5F39CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D846DC-6432-4E27-BC34-9080AA769848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{7A352862-23CD-45AA-9DFF-F661B1D99BB0}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="28800" windowHeight="15370" xr2:uid="{7A352862-23CD-45AA-9DFF-F661B1D99BB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1553,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7349F1CE-6A5E-497A-9668-311349BFBAD7}">
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3836,17 +3836,6 @@
       <c r="N51">
         <v>64</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="M52"/>
-      <c r="N52"/>
-    </row>
-    <row r="53" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="M53"/>
-      <c r="N53"/>
-    </row>
-    <row r="54" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="N54"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>